<commit_message>
update code with varying atmospheric dC13
</commit_message>
<xml_diff>
--- a/mean-pCO2.xlsx
+++ b/mean-pCO2.xlsx
@@ -494,7 +494,7 @@
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="1"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
@@ -515,13 +515,13 @@
         <v>4</v>
       </c>
       <c r="B2" t="n">
-        <v>672.145191867771</v>
+        <v>923.973760067407</v>
       </c>
       <c r="C2" t="n">
-        <v>721.824327957247</v>
+        <v>960.823954066906</v>
       </c>
       <c r="D2" t="n">
-        <v>767.603552296177</v>
+        <v>998.810916723793</v>
       </c>
     </row>
     <row r="3">
@@ -529,13 +529,13 @@
         <v>5</v>
       </c>
       <c r="B3" t="n">
-        <v>425.800156919606</v>
+        <v>559.783827583381</v>
       </c>
       <c r="C3" t="n">
-        <v>458.079993787247</v>
+        <v>582.118385317841</v>
       </c>
       <c r="D3" t="n">
-        <v>488.197306234718</v>
+        <v>605.362998883686</v>
       </c>
     </row>
     <row r="4">
@@ -543,13 +543,13 @@
         <v>6</v>
       </c>
       <c r="B4" t="n">
-        <v>301.144124905283</v>
+        <v>397.931310965265</v>
       </c>
       <c r="C4" t="n">
-        <v>325.912838058545</v>
+        <v>415.387327022327</v>
       </c>
       <c r="D4" t="n">
-        <v>348.530909958238</v>
+        <v>433.212304457446</v>
       </c>
     </row>
     <row r="5">
@@ -557,13 +557,13 @@
         <v>7</v>
       </c>
       <c r="B5" t="n">
-        <v>429.010868192557</v>
+        <v>588.122842069787</v>
       </c>
       <c r="C5" t="n">
-        <v>462.95348436556</v>
+        <v>613.305531535168</v>
       </c>
       <c r="D5" t="n">
-        <v>493.360074575309</v>
+        <v>639.099596511677</v>
       </c>
     </row>
     <row r="6">
@@ -571,13 +571,13 @@
         <v>8</v>
       </c>
       <c r="B6" t="n">
-        <v>1026.03465604002</v>
+        <v>1542.24568071443</v>
       </c>
       <c r="C6" t="n">
-        <v>1101.65115804906</v>
+        <v>1609.85012307864</v>
       </c>
       <c r="D6" t="n">
-        <v>1171.20968044125</v>
+        <v>1680.18343135122</v>
       </c>
     </row>
     <row r="7">
@@ -585,13 +585,13 @@
         <v>9</v>
       </c>
       <c r="B7" t="n">
-        <v>695.799622988916</v>
+        <v>1006.49906226238</v>
       </c>
       <c r="C7" t="n">
-        <v>748.226900495757</v>
+        <v>1049.00596452673</v>
       </c>
       <c r="D7" t="n">
-        <v>796.834966957998</v>
+        <v>1093.92993999406</v>
       </c>
     </row>
     <row r="8">
@@ -599,13 +599,13 @@
         <v>10</v>
       </c>
       <c r="B8" t="n">
-        <v>718.115872845622</v>
+        <v>1028.7754794637</v>
       </c>
       <c r="C8" t="n">
-        <v>772.028712686493</v>
+        <v>1071.34993939978</v>
       </c>
       <c r="D8" t="n">
-        <v>821.860198293902</v>
+        <v>1116.37985239907</v>
       </c>
     </row>
     <row r="9">
@@ -613,13 +613,13 @@
         <v>11</v>
       </c>
       <c r="B9" t="n">
-        <v>421.094063623731</v>
+        <v>561.625330553576</v>
       </c>
       <c r="C9" t="n">
-        <v>453.423098683432</v>
+        <v>584.853320384314</v>
       </c>
       <c r="D9" t="n">
-        <v>483.482639583542</v>
+        <v>608.694667737826</v>
       </c>
     </row>
     <row r="10">
@@ -627,13 +627,13 @@
         <v>12</v>
       </c>
       <c r="B10" t="n">
-        <v>402.832050504757</v>
+        <v>497.845511044643</v>
       </c>
       <c r="C10" t="n">
-        <v>432.334782223552</v>
+        <v>516.143730405052</v>
       </c>
       <c r="D10" t="n">
-        <v>459.61261084743</v>
+        <v>535.260103426921</v>
       </c>
     </row>
     <row r="11">
@@ -641,13 +641,13 @@
         <v>13</v>
       </c>
       <c r="B11" t="n">
-        <v>1079.0387858614</v>
+        <v>1322.37175655249</v>
       </c>
       <c r="C11" t="n">
-        <v>1154.79025582992</v>
+        <v>1370.09782276108</v>
       </c>
       <c r="D11" t="n">
-        <v>1227.40439903262</v>
+        <v>1420.50868107098</v>
       </c>
     </row>
     <row r="12">
@@ -655,13 +655,13 @@
         <v>14</v>
       </c>
       <c r="B12" t="n">
-        <v>1402.67245358751</v>
+        <v>1708.00988975795</v>
       </c>
       <c r="C12" t="n">
-        <v>1499.65308030948</v>
+        <v>1771.26799440878</v>
       </c>
       <c r="D12" t="n">
-        <v>1594.67243085527</v>
+        <v>1833.48231354172</v>
       </c>
     </row>
     <row r="13">
@@ -669,13 +669,13 @@
         <v>15</v>
       </c>
       <c r="B13" t="n">
-        <v>1344.34347845624</v>
+        <v>1690.7195966364</v>
       </c>
       <c r="C13" t="n">
-        <v>1438.2099888986</v>
+        <v>1755.34405300724</v>
       </c>
       <c r="D13" t="n">
-        <v>1529.11941063185</v>
+        <v>1821.10807997118</v>
       </c>
     </row>
     <row r="14">
@@ -683,13 +683,13 @@
         <v>16</v>
       </c>
       <c r="B14" t="n">
-        <v>462.59646650473</v>
+        <v>715.356245312547</v>
       </c>
       <c r="C14" t="n">
-        <v>495.123358685233</v>
+        <v>740.451219575673</v>
       </c>
       <c r="D14" t="n">
-        <v>526.700465983476</v>
+        <v>768.019637080931</v>
       </c>
     </row>
     <row r="15">
@@ -697,13 +697,13 @@
         <v>17</v>
       </c>
       <c r="B15" t="n">
-        <v>856.818023192396</v>
+        <v>1568.34510052532</v>
       </c>
       <c r="C15" t="n">
-        <v>917.071767244109</v>
+        <v>1629.20004467135</v>
       </c>
       <c r="D15" t="n">
-        <v>974.614092237565</v>
+        <v>1693.34751985258</v>
       </c>
     </row>
     <row r="16">
@@ -739,13 +739,13 @@
         <v>20</v>
       </c>
       <c r="B18" t="n">
-        <v>324.707952910247</v>
+        <v>337.568877314667</v>
       </c>
       <c r="C18" t="n">
-        <v>347.887473782663</v>
+        <v>349.374525473069</v>
       </c>
       <c r="D18" t="n">
-        <v>369.872556214638</v>
+        <v>362.260399109824</v>
       </c>
     </row>
     <row r="19">
@@ -753,13 +753,13 @@
         <v>21</v>
       </c>
       <c r="B19" t="n">
-        <v>319.332405715382</v>
+        <v>331.858520281034</v>
       </c>
       <c r="C19" t="n">
-        <v>342.038739526879</v>
+        <v>343.488077431201</v>
       </c>
       <c r="D19" t="n">
-        <v>363.76057701916</v>
+        <v>356.069062827635</v>
       </c>
     </row>
     <row r="20">
@@ -767,13 +767,13 @@
         <v>22</v>
       </c>
       <c r="B20" t="n">
-        <v>1300.44424493369</v>
+        <v>1353.67544427525</v>
       </c>
       <c r="C20" t="n">
-        <v>1388.15744968783</v>
+        <v>1400.89527054604</v>
       </c>
       <c r="D20" t="n">
-        <v>1475.83927502451</v>
+        <v>1447.54089147549</v>
       </c>
     </row>
     <row r="21">
@@ -781,13 +781,13 @@
         <v>23</v>
       </c>
       <c r="B21" t="n">
-        <v>1401.71064474726</v>
+        <v>1241.8720268132</v>
       </c>
       <c r="C21" t="n">
-        <v>1496.93901007639</v>
+        <v>1325.66105255564</v>
       </c>
       <c r="D21" t="n">
-        <v>1591.71540818648</v>
+        <v>1409.40187474181</v>
       </c>
     </row>
     <row r="22">
@@ -963,13 +963,13 @@
         <v>36</v>
       </c>
       <c r="B34" t="n">
-        <v>586.805310854442</v>
+        <v>612.227708648336</v>
       </c>
       <c r="C34" t="n">
-        <v>628.423292331065</v>
+        <v>634.092352518965</v>
       </c>
       <c r="D34" t="n">
-        <v>668.148766045992</v>
+        <v>656.859669754555</v>
       </c>
     </row>
     <row r="35">
@@ -977,13 +977,13 @@
         <v>37</v>
       </c>
       <c r="B35" t="n">
-        <v>1224.57007937737</v>
+        <v>1275.39937290022</v>
       </c>
       <c r="C35" t="n">
-        <v>1307.50653506237</v>
+        <v>1319.89090480613</v>
       </c>
       <c r="D35" t="n">
-        <v>1390.06554405149</v>
+        <v>1364.09319486421</v>
       </c>
     </row>
     <row r="36">
@@ -991,13 +991,13 @@
         <v>38</v>
       </c>
       <c r="B36" t="n">
-        <v>988.541480227917</v>
+        <v>1031.86648405706</v>
       </c>
       <c r="C36" t="n">
-        <v>1057.28669257547</v>
+        <v>1067.93334209049</v>
       </c>
       <c r="D36" t="n">
-        <v>1124.08377091336</v>
+        <v>1104.37822322101</v>
       </c>
     </row>
     <row r="37">
@@ -1005,13 +1005,13 @@
         <v>39</v>
       </c>
       <c r="B37" t="n">
-        <v>624.607016913018</v>
+        <v>651.034799875977</v>
       </c>
       <c r="C37" t="n">
-        <v>668.387796167236</v>
+        <v>673.97634879877</v>
       </c>
       <c r="D37" t="n">
-        <v>710.542862224329</v>
+        <v>697.738722382665</v>
       </c>
     </row>
     <row r="38">
@@ -1019,13 +1019,13 @@
         <v>40</v>
       </c>
       <c r="B38" t="n">
-        <v>1167.31163889477</v>
+        <v>1219.38732176401</v>
       </c>
       <c r="C38" t="n">
-        <v>1248.0849102799</v>
+        <v>1261.99626698928</v>
       </c>
       <c r="D38" t="n">
-        <v>1327.19884935863</v>
+        <v>1305.4367814734</v>
       </c>
     </row>
     <row r="39">
@@ -1033,13 +1033,13 @@
         <v>41</v>
       </c>
       <c r="B39" t="n">
-        <v>1199.94435094563</v>
+        <v>1254.97040039792</v>
       </c>
       <c r="C39" t="n">
-        <v>1283.38183850934</v>
+        <v>1299.88411837301</v>
       </c>
       <c r="D39" t="n">
-        <v>1364.45501689622</v>
+        <v>1345.77898417785</v>
       </c>
     </row>
     <row r="40">
@@ -1047,13 +1047,13 @@
         <v>42</v>
       </c>
       <c r="B40" t="n">
-        <v>999.233512560061</v>
+        <v>1043.613719066</v>
       </c>
       <c r="C40" t="n">
-        <v>1068.7002449554</v>
+        <v>1080.31110102599</v>
       </c>
       <c r="D40" t="n">
-        <v>1136.25815377766</v>
+        <v>1118.0023990411</v>
       </c>
     </row>
     <row r="41">
@@ -1061,13 +1061,13 @@
         <v>43</v>
       </c>
       <c r="B41" t="n">
-        <v>1086.378865416</v>
+        <v>1135.52488546018</v>
       </c>
       <c r="C41" t="n">
-        <v>1162.00221962045</v>
+        <v>1176.16187040954</v>
       </c>
       <c r="D41" t="n">
-        <v>1235.41164975642</v>
+        <v>1217.41229936834</v>
       </c>
     </row>
     <row r="42">
@@ -1075,13 +1075,13 @@
         <v>44</v>
       </c>
       <c r="B42" t="n">
-        <v>1086.67942960109</v>
+        <v>1137.87387493437</v>
       </c>
       <c r="C42" t="n">
-        <v>1162.96706304038</v>
+        <v>1178.92246782829</v>
       </c>
       <c r="D42" t="n">
-        <v>1236.09494849638</v>
+        <v>1220.67015991117</v>
       </c>
     </row>
     <row r="43">
@@ -1089,13 +1089,13 @@
         <v>45</v>
       </c>
       <c r="B43" t="n">
-        <v>332.076125448985</v>
+        <v>467.610477982569</v>
       </c>
       <c r="C43" t="n">
-        <v>356.275064473315</v>
+        <v>484.546787284086</v>
       </c>
       <c r="D43" t="n">
-        <v>378.840753464701</v>
+        <v>502.281855579925</v>
       </c>
     </row>
     <row r="44">
@@ -1103,13 +1103,13 @@
         <v>46</v>
       </c>
       <c r="B44" t="n">
-        <v>669.977401352135</v>
+        <v>969.533946813934</v>
       </c>
       <c r="C44" t="n">
-        <v>715.828940647852</v>
+        <v>1003.83874977954</v>
       </c>
       <c r="D44" t="n">
-        <v>761.302439043239</v>
+        <v>1039.17548430272</v>
       </c>
     </row>
     <row r="45">
@@ -1117,13 +1117,13 @@
         <v>47</v>
       </c>
       <c r="B45" t="n">
-        <v>894.940261504246</v>
+        <v>1518.34678063749</v>
       </c>
       <c r="C45" t="n">
-        <v>957.517112291871</v>
+        <v>1577.18673749734</v>
       </c>
       <c r="D45" t="n">
-        <v>1017.98517005233</v>
+        <v>1637.44424346316</v>
       </c>
     </row>
     <row r="46">
@@ -1131,13 +1131,13 @@
         <v>48</v>
       </c>
       <c r="B46" t="n">
-        <v>890.845169634527</v>
+        <v>1511.35217350176</v>
       </c>
       <c r="C46" t="n">
-        <v>953.166454364625</v>
+        <v>1570.03183084791</v>
       </c>
       <c r="D46" t="n">
-        <v>1013.34471068493</v>
+        <v>1629.99701871238</v>
       </c>
     </row>
     <row r="47">
@@ -1145,13 +1145,13 @@
         <v>49</v>
       </c>
       <c r="B47" t="n">
-        <v>501.705525390107</v>
+        <v>629.992140143226</v>
       </c>
       <c r="C47" t="n">
-        <v>537.648555708929</v>
+        <v>652.45645432786</v>
       </c>
       <c r="D47" t="n">
-        <v>571.714493412499</v>
+        <v>676.359905022304</v>
       </c>
     </row>
     <row r="48">
@@ -1159,13 +1159,13 @@
         <v>50</v>
       </c>
       <c r="B48" t="n">
-        <v>439.365584377949</v>
+        <v>527.289177059437</v>
       </c>
       <c r="C48" t="n">
-        <v>470.129186837702</v>
+        <v>545.898607744204</v>
       </c>
       <c r="D48" t="n">
-        <v>499.816368497413</v>
+        <v>565.086572779063</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
rerun with 0.1 steps in d13Ca
</commit_message>
<xml_diff>
--- a/mean-pCO2.xlsx
+++ b/mean-pCO2.xlsx
@@ -515,13 +515,13 @@
         <v>4</v>
       </c>
       <c r="B2" t="n">
-        <v>923.973760067407</v>
+        <v>935.290659859767</v>
       </c>
       <c r="C2" t="n">
-        <v>960.823954066906</v>
+        <v>949.169319930612</v>
       </c>
       <c r="D2" t="n">
-        <v>998.810916723793</v>
+        <v>962.7163197101</v>
       </c>
     </row>
     <row r="3">
@@ -529,13 +529,13 @@
         <v>5</v>
       </c>
       <c r="B3" t="n">
-        <v>559.783827583381</v>
+        <v>568.741523200579</v>
       </c>
       <c r="C3" t="n">
-        <v>582.118385317841</v>
+        <v>577.24063493066</v>
       </c>
       <c r="D3" t="n">
-        <v>605.362998883686</v>
+        <v>585.503102937956</v>
       </c>
     </row>
     <row r="4">
@@ -543,13 +543,13 @@
         <v>6</v>
       </c>
       <c r="B4" t="n">
-        <v>397.931310965265</v>
+        <v>405.449306488627</v>
       </c>
       <c r="C4" t="n">
-        <v>415.387327022327</v>
+        <v>411.817135020407</v>
       </c>
       <c r="D4" t="n">
-        <v>433.212304457446</v>
+        <v>418.124684501686</v>
       </c>
     </row>
     <row r="5">
@@ -557,13 +557,13 @@
         <v>7</v>
       </c>
       <c r="B5" t="n">
-        <v>588.122842069787</v>
+        <v>596.878222110257</v>
       </c>
       <c r="C5" t="n">
-        <v>613.305531535168</v>
+        <v>606.125156226542</v>
       </c>
       <c r="D5" t="n">
-        <v>639.099596511677</v>
+        <v>615.300270160788</v>
       </c>
     </row>
     <row r="6">
@@ -571,13 +571,13 @@
         <v>8</v>
       </c>
       <c r="B6" t="n">
-        <v>1542.24568071443</v>
+        <v>1550.36215238271</v>
       </c>
       <c r="C6" t="n">
-        <v>1609.85012307864</v>
+        <v>1574.42134302359</v>
       </c>
       <c r="D6" t="n">
-        <v>1680.18343135122</v>
+        <v>1598.57951744317</v>
       </c>
     </row>
     <row r="7">
@@ -585,13 +585,13 @@
         <v>9</v>
       </c>
       <c r="B7" t="n">
-        <v>1006.49906226238</v>
+        <v>1015.33696272899</v>
       </c>
       <c r="C7" t="n">
-        <v>1049.00596452673</v>
+        <v>1030.93628594516</v>
       </c>
       <c r="D7" t="n">
-        <v>1093.92993999406</v>
+        <v>1046.45769364481</v>
       </c>
     </row>
     <row r="8">
@@ -599,13 +599,13 @@
         <v>10</v>
       </c>
       <c r="B8" t="n">
-        <v>1028.7754794637</v>
+        <v>1038.24408157393</v>
       </c>
       <c r="C8" t="n">
-        <v>1071.34993939978</v>
+        <v>1054.05502725735</v>
       </c>
       <c r="D8" t="n">
-        <v>1116.37985239907</v>
+        <v>1069.78613018249</v>
       </c>
     </row>
     <row r="9">
@@ -613,13 +613,13 @@
         <v>11</v>
       </c>
       <c r="B9" t="n">
-        <v>561.625330553576</v>
+        <v>570.65040444965</v>
       </c>
       <c r="C9" t="n">
-        <v>584.853320384314</v>
+        <v>579.295446297309</v>
       </c>
       <c r="D9" t="n">
-        <v>608.694667737826</v>
+        <v>587.817459887338</v>
       </c>
     </row>
     <row r="10">
@@ -627,13 +627,13 @@
         <v>12</v>
       </c>
       <c r="B10" t="n">
-        <v>497.845511044643</v>
+        <v>506.73124574577</v>
       </c>
       <c r="C10" t="n">
-        <v>516.143730405052</v>
+        <v>513.831042510357</v>
       </c>
       <c r="D10" t="n">
-        <v>535.260103426921</v>
+        <v>520.797065883371</v>
       </c>
     </row>
     <row r="11">
@@ -641,13 +641,13 @@
         <v>13</v>
       </c>
       <c r="B11" t="n">
-        <v>1322.37175655249</v>
+        <v>1339.97480409885</v>
       </c>
       <c r="C11" t="n">
-        <v>1370.09782276108</v>
+        <v>1358.65567204488</v>
       </c>
       <c r="D11" t="n">
-        <v>1420.50868107098</v>
+        <v>1376.88614226082</v>
       </c>
     </row>
     <row r="12">
@@ -655,13 +655,13 @@
         <v>14</v>
       </c>
       <c r="B12" t="n">
-        <v>1708.00988975795</v>
+        <v>1733.40878562539</v>
       </c>
       <c r="C12" t="n">
-        <v>1771.26799440878</v>
+        <v>1757.22872000623</v>
       </c>
       <c r="D12" t="n">
-        <v>1833.48231354172</v>
+        <v>1780.37500308953</v>
       </c>
     </row>
     <row r="13">
@@ -669,13 +669,13 @@
         <v>15</v>
       </c>
       <c r="B13" t="n">
-        <v>1690.7195966364</v>
+        <v>1711.50828778401</v>
       </c>
       <c r="C13" t="n">
-        <v>1755.34405300724</v>
+        <v>1735.56134366754</v>
       </c>
       <c r="D13" t="n">
-        <v>1821.10807997118</v>
+        <v>1759.5505181623</v>
       </c>
     </row>
     <row r="14">
@@ -683,13 +683,13 @@
         <v>16</v>
       </c>
       <c r="B14" t="n">
-        <v>715.356245312547</v>
+        <v>725.783565027881</v>
       </c>
       <c r="C14" t="n">
-        <v>740.451219575673</v>
+        <v>735.966090869871</v>
       </c>
       <c r="D14" t="n">
-        <v>768.019637080931</v>
+        <v>745.981402973445</v>
       </c>
     </row>
     <row r="15">
@@ -697,13 +697,13 @@
         <v>17</v>
       </c>
       <c r="B15" t="n">
-        <v>1568.34510052532</v>
+        <v>1582.97567315157</v>
       </c>
       <c r="C15" t="n">
-        <v>1629.20004467135</v>
+        <v>1605.85287299653</v>
       </c>
       <c r="D15" t="n">
-        <v>1693.34751985258</v>
+        <v>1628.85458982247</v>
       </c>
     </row>
     <row r="16">
@@ -711,13 +711,13 @@
         <v>18</v>
       </c>
       <c r="B16" t="n">
-        <v>360.229381501604</v>
+        <v>363.104338666042</v>
       </c>
       <c r="C16" t="n">
         <v>386.518765738998</v>
       </c>
       <c r="D16" t="n">
-        <v>411.139610706897</v>
+        <v>410.37950110092</v>
       </c>
     </row>
     <row r="17">
@@ -725,13 +725,13 @@
         <v>19</v>
       </c>
       <c r="B17" t="n">
-        <v>358.635997884421</v>
+        <v>361.192176919612</v>
       </c>
       <c r="C17" t="n">
         <v>384.315901788441</v>
       </c>
       <c r="D17" t="n">
-        <v>408.741111410945</v>
+        <v>408.017517394318</v>
       </c>
     </row>
     <row r="18">
@@ -739,13 +739,13 @@
         <v>20</v>
       </c>
       <c r="B18" t="n">
-        <v>337.568877314667</v>
+        <v>344.078450239495</v>
       </c>
       <c r="C18" t="n">
-        <v>349.374525473069</v>
+        <v>348.703558933792</v>
       </c>
       <c r="D18" t="n">
-        <v>362.260399109824</v>
+        <v>353.296371475418</v>
       </c>
     </row>
     <row r="19">
@@ -753,13 +753,13 @@
         <v>21</v>
       </c>
       <c r="B19" t="n">
-        <v>331.858520281034</v>
+        <v>338.292076804077</v>
       </c>
       <c r="C19" t="n">
-        <v>343.488077431201</v>
+        <v>342.834142773817</v>
       </c>
       <c r="D19" t="n">
-        <v>356.069062827635</v>
+        <v>347.349050052238</v>
       </c>
     </row>
     <row r="20">
@@ -767,13 +767,13 @@
         <v>22</v>
       </c>
       <c r="B20" t="n">
-        <v>1353.67544427525</v>
+        <v>1376.56165587883</v>
       </c>
       <c r="C20" t="n">
-        <v>1400.89527054604</v>
+        <v>1395.1302780526</v>
       </c>
       <c r="D20" t="n">
-        <v>1447.54089147549</v>
+        <v>1412.94255690797</v>
       </c>
     </row>
     <row r="21">
@@ -781,13 +781,13 @@
         <v>23</v>
       </c>
       <c r="B21" t="n">
-        <v>1241.8720268132</v>
+        <v>1248.63776891335</v>
       </c>
       <c r="C21" t="n">
         <v>1325.66105255564</v>
       </c>
       <c r="D21" t="n">
-        <v>1409.40187474181</v>
+        <v>1403.15897493905</v>
       </c>
     </row>
     <row r="22">
@@ -795,13 +795,13 @@
         <v>24</v>
       </c>
       <c r="B22" t="n">
-        <v>1225.40138749385</v>
+        <v>1233.28110469582</v>
       </c>
       <c r="C22" t="n">
         <v>1309.95720885714</v>
       </c>
       <c r="D22" t="n">
-        <v>1393.39459316027</v>
+        <v>1386.97917326292</v>
       </c>
     </row>
     <row r="23">
@@ -809,13 +809,13 @@
         <v>25</v>
       </c>
       <c r="B23" t="n">
-        <v>1425.92625478313</v>
+        <v>1434.99123686254</v>
       </c>
       <c r="C23" t="n">
         <v>1524.24186187738</v>
       </c>
       <c r="D23" t="n">
-        <v>1620.87875375749</v>
+        <v>1613.45865931237</v>
       </c>
     </row>
     <row r="24">
@@ -823,13 +823,13 @@
         <v>26</v>
       </c>
       <c r="B24" t="n">
-        <v>1420.01479991557</v>
+        <v>1429.82896658252</v>
       </c>
       <c r="C24" t="n">
         <v>1519.38723988872</v>
       </c>
       <c r="D24" t="n">
-        <v>1615.08183510329</v>
+        <v>1610.76678453751</v>
       </c>
     </row>
     <row r="25">
@@ -837,13 +837,13 @@
         <v>27</v>
       </c>
       <c r="B25" t="n">
-        <v>1810.96794702506</v>
+        <v>1822.41332470373</v>
       </c>
       <c r="C25" t="n">
         <v>1935.83446574227</v>
       </c>
       <c r="D25" t="n">
-        <v>2059.03132316216</v>
+        <v>2049.37076748755</v>
       </c>
     </row>
     <row r="26">
@@ -851,13 +851,13 @@
         <v>28</v>
       </c>
       <c r="B26" t="n">
-        <v>1367.77243899644</v>
+        <v>1376.17814789472</v>
       </c>
       <c r="C26" t="n">
         <v>1461.219787589</v>
       </c>
       <c r="D26" t="n">
-        <v>1553.47344293772</v>
+        <v>1546.77875310165</v>
       </c>
     </row>
     <row r="27">
@@ -865,13 +865,13 @@
         <v>29</v>
       </c>
       <c r="B27" t="n">
-        <v>1179.31428981552</v>
+        <v>1186.84177505301</v>
       </c>
       <c r="C27" t="n">
         <v>1260.64927057516</v>
       </c>
       <c r="D27" t="n">
-        <v>1340.54598528014</v>
+        <v>1334.36353390158</v>
       </c>
     </row>
     <row r="28">
@@ -879,13 +879,13 @@
         <v>30</v>
       </c>
       <c r="B28" t="n">
-        <v>2439.8994117427</v>
+        <v>2456.61564790846</v>
       </c>
       <c r="C28" t="n">
         <v>2609.65167710147</v>
       </c>
       <c r="D28" t="n">
-        <v>2774.14505946803</v>
+        <v>2764.24264881697</v>
       </c>
     </row>
     <row r="29">
@@ -893,13 +893,13 @@
         <v>31</v>
       </c>
       <c r="B29" t="n">
-        <v>2425.12088859715</v>
+        <v>2441.74301581139</v>
       </c>
       <c r="C29" t="n">
         <v>2593.86668542891</v>
       </c>
       <c r="D29" t="n">
-        <v>2757.34745222281</v>
+        <v>2747.69901887352</v>
       </c>
     </row>
     <row r="30">
@@ -907,13 +907,13 @@
         <v>32</v>
       </c>
       <c r="B30" t="n">
-        <v>2101.08849215256</v>
+        <v>2114.03843865272</v>
       </c>
       <c r="C30" t="n">
         <v>2245.5202463693</v>
       </c>
       <c r="D30" t="n">
-        <v>2388.62998541453</v>
+        <v>2377.00712085549</v>
       </c>
     </row>
     <row r="31">
@@ -921,13 +921,13 @@
         <v>33</v>
       </c>
       <c r="B31" t="n">
-        <v>2038.76446630811</v>
+        <v>2052.81004074937</v>
       </c>
       <c r="C31" t="n">
         <v>2180.63003630976</v>
       </c>
       <c r="D31" t="n">
-        <v>2318.10028149289</v>
+        <v>2309.53984380317</v>
       </c>
     </row>
     <row r="32">
@@ -935,13 +935,13 @@
         <v>34</v>
       </c>
       <c r="B32" t="n">
-        <v>479.825186555014</v>
+        <v>482.911910649433</v>
       </c>
       <c r="C32" t="n">
         <v>513.164977530873</v>
       </c>
       <c r="D32" t="n">
-        <v>545.883850747776</v>
+        <v>544.071426909266</v>
       </c>
     </row>
     <row r="33">
@@ -949,13 +949,13 @@
         <v>35</v>
       </c>
       <c r="B33" t="n">
-        <v>514.722530056837</v>
+        <v>518.207769602502</v>
       </c>
       <c r="C33" t="n">
         <v>550.91137315916</v>
       </c>
       <c r="D33" t="n">
-        <v>586.039668518835</v>
+        <v>584.43443412136</v>
       </c>
     </row>
     <row r="34">
@@ -963,13 +963,13 @@
         <v>36</v>
       </c>
       <c r="B34" t="n">
-        <v>612.227708648336</v>
+        <v>622.976314845446</v>
       </c>
       <c r="C34" t="n">
-        <v>634.092352518965</v>
+        <v>631.526849583293</v>
       </c>
       <c r="D34" t="n">
-        <v>656.859669754555</v>
+        <v>639.863940396487</v>
       </c>
     </row>
     <row r="35">
@@ -977,13 +977,13 @@
         <v>37</v>
       </c>
       <c r="B35" t="n">
-        <v>1275.39937290022</v>
+        <v>1296.7410188606</v>
       </c>
       <c r="C35" t="n">
-        <v>1319.89090480613</v>
+        <v>1314.28484770269</v>
       </c>
       <c r="D35" t="n">
-        <v>1364.09319486421</v>
+        <v>1331.04306246265</v>
       </c>
     </row>
     <row r="36">
@@ -991,13 +991,13 @@
         <v>38</v>
       </c>
       <c r="B36" t="n">
-        <v>1031.86648405706</v>
+        <v>1048.92930777992</v>
       </c>
       <c r="C36" t="n">
-        <v>1067.93334209049</v>
+        <v>1063.1121073411</v>
       </c>
       <c r="D36" t="n">
-        <v>1104.37822322101</v>
+        <v>1076.78196780946</v>
       </c>
     </row>
     <row r="37">
@@ -1005,13 +1005,13 @@
         <v>39</v>
       </c>
       <c r="B37" t="n">
-        <v>651.034799875977</v>
+        <v>662.485296933878</v>
       </c>
       <c r="C37" t="n">
-        <v>673.97634879877</v>
+        <v>671.44831876705</v>
       </c>
       <c r="D37" t="n">
-        <v>697.738722382665</v>
+        <v>680.238923676199</v>
       </c>
     </row>
     <row r="38">
@@ -1019,13 +1019,13 @@
         <v>40</v>
       </c>
       <c r="B38" t="n">
-        <v>1219.38732176401</v>
+        <v>1238.84515417432</v>
       </c>
       <c r="C38" t="n">
-        <v>1261.99626698928</v>
+        <v>1255.69241748671</v>
       </c>
       <c r="D38" t="n">
-        <v>1305.4367814734</v>
+        <v>1271.92305723476</v>
       </c>
     </row>
     <row r="39">
@@ -1033,13 +1033,13 @@
         <v>41</v>
       </c>
       <c r="B39" t="n">
-        <v>1254.97040039792</v>
+        <v>1274.97115761175</v>
       </c>
       <c r="C39" t="n">
-        <v>1299.88411837301</v>
+        <v>1292.39824074298</v>
       </c>
       <c r="D39" t="n">
-        <v>1345.77898417785</v>
+        <v>1309.19394878223</v>
       </c>
     </row>
     <row r="40">
@@ -1047,13 +1047,13 @@
         <v>42</v>
       </c>
       <c r="B40" t="n">
-        <v>1043.613719066</v>
+        <v>1060.590484961</v>
       </c>
       <c r="C40" t="n">
-        <v>1080.31110102599</v>
+        <v>1075.05063274154</v>
       </c>
       <c r="D40" t="n">
-        <v>1118.0023990411</v>
+        <v>1088.94904150001</v>
       </c>
     </row>
     <row r="41">
@@ -1061,13 +1061,13 @@
         <v>43</v>
       </c>
       <c r="B41" t="n">
-        <v>1135.52488546018</v>
+        <v>1153.89012402349</v>
       </c>
       <c r="C41" t="n">
-        <v>1176.16187040954</v>
+        <v>1169.74135892255</v>
       </c>
       <c r="D41" t="n">
-        <v>1217.41229936834</v>
+        <v>1184.9359618325</v>
       </c>
     </row>
     <row r="42">
@@ -1075,13 +1075,13 @@
         <v>44</v>
       </c>
       <c r="B42" t="n">
-        <v>1137.87387493437</v>
+        <v>1155.88669322891</v>
       </c>
       <c r="C42" t="n">
-        <v>1178.92246782829</v>
+        <v>1171.68079542622</v>
       </c>
       <c r="D42" t="n">
-        <v>1220.67015991117</v>
+        <v>1187.01288409883</v>
       </c>
     </row>
     <row r="43">
@@ -1089,13 +1089,13 @@
         <v>45</v>
       </c>
       <c r="B43" t="n">
-        <v>467.610477982569</v>
+        <v>475.938908636944</v>
       </c>
       <c r="C43" t="n">
-        <v>484.546787284086</v>
+        <v>482.592326589112</v>
       </c>
       <c r="D43" t="n">
-        <v>502.281855579925</v>
+        <v>489.115085178555</v>
       </c>
     </row>
     <row r="44">
@@ -1103,13 +1103,13 @@
         <v>46</v>
       </c>
       <c r="B44" t="n">
-        <v>969.533946813934</v>
+        <v>985.323396438844</v>
       </c>
       <c r="C44" t="n">
-        <v>1003.83874977954</v>
+        <v>998.816007626036</v>
       </c>
       <c r="D44" t="n">
-        <v>1039.17548430272</v>
+        <v>1011.80621379709</v>
       </c>
     </row>
     <row r="45">
@@ -1117,13 +1117,13 @@
         <v>47</v>
       </c>
       <c r="B45" t="n">
-        <v>1518.34678063749</v>
+        <v>1535.70254052128</v>
       </c>
       <c r="C45" t="n">
-        <v>1577.18673749734</v>
+        <v>1557.56182306632</v>
       </c>
       <c r="D45" t="n">
-        <v>1637.44424346316</v>
+        <v>1579.39986834752</v>
       </c>
     </row>
     <row r="46">
@@ -1131,13 +1131,13 @@
         <v>48</v>
       </c>
       <c r="B46" t="n">
-        <v>1511.35217350176</v>
+        <v>1528.77883144404</v>
       </c>
       <c r="C46" t="n">
-        <v>1570.03183084791</v>
+        <v>1550.49528063082</v>
       </c>
       <c r="D46" t="n">
-        <v>1629.99701871238</v>
+        <v>1572.25264980169</v>
       </c>
     </row>
     <row r="47">
@@ -1145,13 +1145,13 @@
         <v>49</v>
       </c>
       <c r="B47" t="n">
-        <v>629.992140143226</v>
+        <v>639.99697247528</v>
       </c>
       <c r="C47" t="n">
-        <v>652.45645432786</v>
+        <v>648.947715757392</v>
       </c>
       <c r="D47" t="n">
-        <v>676.359905022304</v>
+        <v>657.73179010961</v>
       </c>
     </row>
     <row r="48">
@@ -1159,13 +1159,13 @@
         <v>50</v>
       </c>
       <c r="B48" t="n">
-        <v>527.289177059437</v>
+        <v>536.948656657408</v>
       </c>
       <c r="C48" t="n">
-        <v>545.898607744204</v>
+        <v>544.176543723348</v>
       </c>
       <c r="D48" t="n">
-        <v>565.086572779063</v>
+        <v>551.284137517882</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
calculate highest posterior density interval
</commit_message>
<xml_diff>
--- a/mean-pCO2.xlsx
+++ b/mean-pCO2.xlsx
@@ -515,13 +515,13 @@
         <v>4</v>
       </c>
       <c r="B2" t="n">
-        <v>418.654330938922</v>
+        <v>354.312659315757</v>
       </c>
       <c r="C2" t="n">
         <v>1030.93628594516</v>
       </c>
       <c r="D2" t="n">
-        <v>1965.93572038396</v>
+        <v>1817.7522476787</v>
       </c>
     </row>
     <row r="3">
@@ -529,13 +529,13 @@
         <v>5</v>
       </c>
       <c r="B3" t="n">
-        <v>433.328583997645</v>
+        <v>374.984834279778</v>
       </c>
       <c r="C3" t="n">
         <v>1054.05502725735</v>
       </c>
       <c r="D3" t="n">
-        <v>1990.94409467863</v>
+        <v>1851.59427516284</v>
       </c>
     </row>
     <row r="4">
@@ -543,13 +543,13 @@
         <v>6</v>
       </c>
       <c r="B4" t="n">
-        <v>399.93298639518</v>
+        <v>353.892957746479</v>
       </c>
       <c r="C4" t="n">
         <v>949.169319930612</v>
       </c>
       <c r="D4" t="n">
-        <v>1743.84684599406</v>
+        <v>1630.94332552693</v>
       </c>
     </row>
     <row r="5">
@@ -557,13 +557,13 @@
         <v>7</v>
       </c>
       <c r="B5" t="n">
-        <v>241.574177851094</v>
+        <v>216.137688666002</v>
       </c>
       <c r="C5" t="n">
         <v>577.24063493066</v>
       </c>
       <c r="D5" t="n">
-        <v>1054.03882998917</v>
+        <v>995.22224953073</v>
       </c>
     </row>
     <row r="6">
@@ -571,13 +571,13 @@
         <v>8</v>
       </c>
       <c r="B6" t="n">
-        <v>161.785270430932</v>
+        <v>135.378030604928</v>
       </c>
       <c r="C6" t="n">
         <v>411.817135020407</v>
       </c>
       <c r="D6" t="n">
-        <v>788.415755997504</v>
+        <v>731.123832624966</v>
       </c>
     </row>
     <row r="7">
@@ -585,13 +585,13 @@
         <v>9</v>
       </c>
       <c r="B7" t="n">
-        <v>243.766570654361</v>
+        <v>206.093685390115</v>
       </c>
       <c r="C7" t="n">
         <v>606.125156226542</v>
       </c>
       <c r="D7" t="n">
-        <v>1153.70440069318</v>
+        <v>1067.85681923597</v>
       </c>
     </row>
     <row r="8">
@@ -599,13 +599,13 @@
         <v>10</v>
       </c>
       <c r="B8" t="n">
-        <v>638.839645586087</v>
+        <v>529.340625566246</v>
       </c>
       <c r="C8" t="n">
         <v>1574.42134302359</v>
       </c>
       <c r="D8" t="n">
-        <v>3039.39573066251</v>
+        <v>2782.32020958726</v>
       </c>
     </row>
     <row r="9">
@@ -613,13 +613,13 @@
         <v>11</v>
       </c>
       <c r="B9" t="n">
-        <v>177.626658639482</v>
+        <v>156.569767658106</v>
       </c>
       <c r="C9" t="n">
         <v>386.518765738998</v>
       </c>
       <c r="D9" t="n">
-        <v>647.677126566565</v>
+        <v>604.498651462128</v>
       </c>
     </row>
     <row r="10">
@@ -627,13 +627,13 @@
         <v>12</v>
       </c>
       <c r="B10" t="n">
-        <v>177.146209571236</v>
+        <v>156.845958742782</v>
       </c>
       <c r="C10" t="n">
         <v>384.315901788441</v>
       </c>
       <c r="D10" t="n">
-        <v>641.759403647139</v>
+        <v>598.975443403997</v>
       </c>
     </row>
     <row r="11">
@@ -641,13 +641,13 @@
         <v>13</v>
       </c>
       <c r="B11" t="n">
-        <v>255.804836224378</v>
+        <v>229.669238439386</v>
       </c>
       <c r="C11" t="n">
         <v>550.91137315916</v>
       </c>
       <c r="D11" t="n">
-        <v>909.252326678038</v>
+        <v>851.646775882724</v>
       </c>
     </row>
     <row r="12">
@@ -655,13 +655,13 @@
         <v>14</v>
       </c>
       <c r="B12" t="n">
-        <v>285.212131999635</v>
+        <v>260.363550388584</v>
       </c>
       <c r="C12" t="n">
         <v>631.526849583293</v>
       </c>
       <c r="D12" t="n">
-        <v>1067.77783770637</v>
+        <v>1020.36513260567</v>
       </c>
     </row>
     <row r="13">
@@ -669,13 +669,13 @@
         <v>15</v>
       </c>
       <c r="B13" t="n">
-        <v>489.704486692204</v>
+        <v>449.507402408847</v>
       </c>
       <c r="C13" t="n">
         <v>1063.1121073411</v>
       </c>
       <c r="D13" t="n">
-        <v>1764.68007077721</v>
+        <v>1692.68435682913</v>
       </c>
     </row>
     <row r="14">
@@ -683,13 +683,13 @@
         <v>16</v>
       </c>
       <c r="B14" t="n">
-        <v>306.020730164355</v>
+        <v>280.030289857542</v>
       </c>
       <c r="C14" t="n">
         <v>671.44831876705</v>
       </c>
       <c r="D14" t="n">
-        <v>1124.39770310332</v>
+        <v>1078.96427461686</v>
       </c>
     </row>
     <row r="15">
@@ -697,13 +697,13 @@
         <v>17</v>
       </c>
       <c r="B15" t="n">
-        <v>610.034757176734</v>
+        <v>557.211232419769</v>
       </c>
       <c r="C15" t="n">
         <v>1314.28484770269</v>
       </c>
       <c r="D15" t="n">
-        <v>2158.70528520742</v>
+        <v>2068.78947817386</v>
       </c>
     </row>
     <row r="16">
@@ -711,13 +711,13 @@
         <v>18</v>
       </c>
       <c r="B16" t="n">
-        <v>287.782548587827</v>
+        <v>249.89123999692</v>
       </c>
       <c r="C16" t="n">
         <v>648.947715757392</v>
       </c>
       <c r="D16" t="n">
-        <v>1122.02302701395</v>
+        <v>1058.60754177337</v>
       </c>
     </row>
     <row r="17">
@@ -725,13 +725,13 @@
         <v>19</v>
       </c>
       <c r="B17" t="n">
-        <v>578.303885183693</v>
+        <v>533.363431057008</v>
       </c>
       <c r="C17" t="n">
         <v>1255.69241748671</v>
       </c>
       <c r="D17" t="n">
-        <v>2085.44323252149</v>
+        <v>1999.49913475042</v>
       </c>
     </row>
     <row r="18">
@@ -739,13 +739,13 @@
         <v>20</v>
       </c>
       <c r="B18" t="n">
-        <v>590.864942768758</v>
+        <v>538.942825535404</v>
       </c>
       <c r="C18" t="n">
         <v>1292.39824074298</v>
       </c>
       <c r="D18" t="n">
-        <v>2170.12236157928</v>
+        <v>2072.19980004882</v>
       </c>
     </row>
     <row r="19">
@@ -753,13 +753,13 @@
         <v>21</v>
       </c>
       <c r="B19" t="n">
-        <v>493.577524143013</v>
+        <v>454.347461223283</v>
       </c>
       <c r="C19" t="n">
         <v>1075.05063274154</v>
       </c>
       <c r="D19" t="n">
-        <v>1795.21980408841</v>
+        <v>1720.34194977037</v>
       </c>
     </row>
     <row r="20">
@@ -767,13 +767,13 @@
         <v>22</v>
       </c>
       <c r="B20" t="n">
-        <v>534.590611736301</v>
+        <v>469.525406671454</v>
       </c>
       <c r="C20" t="n">
         <v>1169.74135892255</v>
       </c>
       <c r="D20" t="n">
-        <v>1963.16580589113</v>
+        <v>1854.2900208017</v>
       </c>
     </row>
     <row r="21">
@@ -781,13 +781,13 @@
         <v>23</v>
       </c>
       <c r="B21" t="n">
-        <v>531.280997750162</v>
+        <v>487.296760859198</v>
       </c>
       <c r="C21" t="n">
         <v>1171.68079542622</v>
       </c>
       <c r="D21" t="n">
-        <v>1986.57015058758</v>
+        <v>1895.25200954586</v>
       </c>
     </row>
     <row r="22">
@@ -795,13 +795,13 @@
         <v>24</v>
       </c>
       <c r="B22" t="n">
-        <v>239.644619370009</v>
+        <v>216.81281391383</v>
       </c>
       <c r="C22" t="n">
         <v>513.164977530873</v>
       </c>
       <c r="D22" t="n">
-        <v>837.281858045659</v>
+        <v>791.936239372724</v>
       </c>
     </row>
     <row r="23">
@@ -809,13 +809,13 @@
         <v>25</v>
       </c>
       <c r="B23" t="n">
-        <v>607.341679905819</v>
+        <v>517.766977277684</v>
       </c>
       <c r="C23" t="n">
         <v>1358.65567204488</v>
       </c>
       <c r="D23" t="n">
-        <v>2346.36221431474</v>
+        <v>2191.995183028</v>
       </c>
     </row>
     <row r="24">
@@ -823,13 +823,13 @@
         <v>26</v>
       </c>
       <c r="B24" t="n">
-        <v>791.8368710807</v>
+        <v>715.061720362547</v>
       </c>
       <c r="C24" t="n">
         <v>1757.22872000623</v>
       </c>
       <c r="D24" t="n">
-        <v>2994.40605919296</v>
+        <v>2844.44689668828</v>
       </c>
     </row>
     <row r="25">
@@ -837,13 +837,13 @@
         <v>27</v>
       </c>
       <c r="B25" t="n">
-        <v>763.274891259923</v>
+        <v>667.206057120518</v>
       </c>
       <c r="C25" t="n">
         <v>1735.56134366754</v>
       </c>
       <c r="D25" t="n">
-        <v>3062.09456367895</v>
+        <v>2871.28722931183</v>
       </c>
     </row>
     <row r="26">
@@ -851,13 +851,13 @@
         <v>28</v>
       </c>
       <c r="B26" t="n">
-        <v>326.090853480162</v>
+        <v>289.766781433583</v>
       </c>
       <c r="C26" t="n">
         <v>735.966090869871</v>
       </c>
       <c r="D26" t="n">
-        <v>1275.13683189274</v>
+        <v>1207.68538137971</v>
       </c>
     </row>
     <row r="27">
@@ -865,13 +865,13 @@
         <v>29</v>
       </c>
       <c r="B27" t="n">
-        <v>689.335096825906</v>
+        <v>593.088632108031</v>
       </c>
       <c r="C27" t="n">
         <v>1605.85287299653</v>
       </c>
       <c r="D27" t="n">
-        <v>2919.32203012511</v>
+        <v>2719.41827785334</v>
       </c>
     </row>
     <row r="28">
@@ -879,13 +879,13 @@
         <v>30</v>
       </c>
       <c r="B28" t="n">
-        <v>456.130494743278</v>
+        <v>412.096366237632</v>
       </c>
       <c r="C28" t="n">
         <v>998.816007626036</v>
       </c>
       <c r="D28" t="n">
-        <v>1677.20323719768</v>
+        <v>1597.50328149219</v>
       </c>
     </row>
     <row r="29">
@@ -893,13 +893,13 @@
         <v>31</v>
       </c>
       <c r="B29" t="n">
-        <v>213.87097117414</v>
+        <v>191.279079447917</v>
       </c>
       <c r="C29" t="n">
         <v>482.592326589112</v>
       </c>
       <c r="D29" t="n">
-        <v>833.45512972036</v>
+        <v>792.971626044365</v>
       </c>
     </row>
     <row r="30">
@@ -907,13 +907,13 @@
         <v>32</v>
       </c>
       <c r="B30" t="n">
-        <v>238.497095953367</v>
+        <v>206.221650425231</v>
       </c>
       <c r="C30" t="n">
         <v>579.295446297309</v>
       </c>
       <c r="D30" t="n">
-        <v>1077.49142588147</v>
+        <v>1005.01159361935</v>
       </c>
     </row>
     <row r="31">
@@ -921,13 +921,13 @@
         <v>33</v>
       </c>
       <c r="B31" t="n">
-        <v>226.329868472907</v>
+        <v>203.144630664703</v>
       </c>
       <c r="C31" t="n">
         <v>513.831042510357</v>
       </c>
       <c r="D31" t="n">
-        <v>890.41311044662</v>
+        <v>847.382655260253</v>
       </c>
     </row>
     <row r="32">
@@ -935,13 +935,13 @@
         <v>34</v>
       </c>
       <c r="B32" t="n">
-        <v>709.012932871733</v>
+        <v>645.892587233709</v>
       </c>
       <c r="C32" t="n">
         <v>1519.38723988872</v>
       </c>
       <c r="D32" t="n">
-        <v>2484.50963248083</v>
+        <v>2338.47748702646</v>
       </c>
     </row>
     <row r="33">
@@ -949,13 +949,13 @@
         <v>35</v>
       </c>
       <c r="B33" t="n">
-        <v>911.997277344848</v>
+        <v>841.705442971699</v>
       </c>
       <c r="C33" t="n">
         <v>1935.83446574227</v>
       </c>
       <c r="D33" t="n">
-        <v>3104.19989436216</v>
+        <v>2970.18441440874</v>
       </c>
     </row>
     <row r="34">
@@ -963,13 +963,13 @@
         <v>36</v>
       </c>
       <c r="B34" t="n">
-        <v>693.18751475001</v>
+        <v>660.30475218755</v>
       </c>
       <c r="C34" t="n">
         <v>1461.219787589</v>
       </c>
       <c r="D34" t="n">
-        <v>2308.79760956415</v>
+        <v>2251.361181084</v>
       </c>
     </row>
     <row r="35">
@@ -977,13 +977,13 @@
         <v>37</v>
       </c>
       <c r="B35" t="n">
-        <v>595.594886187156</v>
+        <v>550.505207716531</v>
       </c>
       <c r="C35" t="n">
         <v>1260.64927057516</v>
       </c>
       <c r="D35" t="n">
-        <v>2009.08976353488</v>
+        <v>1934.18646323408</v>
       </c>
     </row>
     <row r="36">
@@ -991,13 +991,13 @@
         <v>38</v>
       </c>
       <c r="B36" t="n">
-        <v>1223.78966446432</v>
+        <v>1124.85721896266</v>
       </c>
       <c r="C36" t="n">
         <v>2609.65167710147</v>
       </c>
       <c r="D36" t="n">
-        <v>4225.8753962172</v>
+        <v>4006.65169540156</v>
       </c>
     </row>
     <row r="37">
@@ -1005,13 +1005,13 @@
         <v>39</v>
       </c>
       <c r="B37" t="n">
-        <v>1217.37489906606</v>
+        <v>1119.98811416649</v>
       </c>
       <c r="C37" t="n">
         <v>2593.86668542891</v>
       </c>
       <c r="D37" t="n">
-        <v>4193.20956348461</v>
+        <v>3981.65866647652</v>
       </c>
     </row>
     <row r="38">
@@ -1019,13 +1019,13 @@
         <v>40</v>
       </c>
       <c r="B38" t="n">
-        <v>1058.74912340918</v>
+        <v>978.755625748932</v>
       </c>
       <c r="C38" t="n">
         <v>2245.5202463693</v>
       </c>
       <c r="D38" t="n">
-        <v>3594.97303905944</v>
+        <v>3443.67624577205</v>
       </c>
     </row>
     <row r="39">
@@ -1033,13 +1033,13 @@
         <v>41</v>
       </c>
       <c r="B39" t="n">
-        <v>1024.67620323366</v>
+        <v>943.291487066612</v>
       </c>
       <c r="C39" t="n">
         <v>2180.63003630976</v>
       </c>
       <c r="D39" t="n">
-        <v>3515.8899927096</v>
+        <v>3347.36304645877</v>
       </c>
     </row>
     <row r="40">
@@ -1047,13 +1047,13 @@
         <v>42</v>
       </c>
       <c r="B40" t="n">
-        <v>719.730508063422</v>
+        <v>665.386291658186</v>
       </c>
       <c r="C40" t="n">
         <v>1524.24186187738</v>
       </c>
       <c r="D40" t="n">
-        <v>2432.22114946767</v>
+        <v>2338.17295116595</v>
       </c>
     </row>
     <row r="41">
@@ -1061,13 +1061,13 @@
         <v>43</v>
       </c>
       <c r="B41" t="n">
-        <v>649.049861490604</v>
+        <v>610.166617640876</v>
       </c>
       <c r="C41" t="n">
         <v>1395.1302780526</v>
       </c>
       <c r="D41" t="n">
-        <v>2286.0169508225</v>
+        <v>2205.05439890485</v>
       </c>
     </row>
     <row r="42">
@@ -1075,13 +1075,13 @@
         <v>44</v>
       </c>
       <c r="B42" t="n">
-        <v>155.40398101238</v>
+        <v>141.581050401698</v>
       </c>
       <c r="C42" t="n">
         <v>342.834142773817</v>
       </c>
       <c r="D42" t="n">
-        <v>575.155334205666</v>
+        <v>552.858823354043</v>
       </c>
     </row>
     <row r="43">
@@ -1089,13 +1089,13 @@
         <v>45</v>
       </c>
       <c r="B43" t="n">
-        <v>158.26305245662</v>
+        <v>144.189712427675</v>
       </c>
       <c r="C43" t="n">
         <v>348.703558933792</v>
       </c>
       <c r="D43" t="n">
-        <v>584.389259721646</v>
+        <v>561.964627310409</v>
       </c>
     </row>
     <row r="44">
@@ -1103,13 +1103,13 @@
         <v>46</v>
       </c>
       <c r="B44" t="n">
-        <v>629.800609374635</v>
+        <v>600.540849909865</v>
       </c>
       <c r="C44" t="n">
         <v>1325.66105255564</v>
       </c>
       <c r="D44" t="n">
-        <v>2088.0135083336</v>
+        <v>2037.62729743552</v>
       </c>
     </row>
     <row r="45">
@@ -1117,13 +1117,13 @@
         <v>47</v>
       </c>
       <c r="B45" t="n">
-        <v>617.492800620922</v>
+        <v>569.196264007643</v>
       </c>
       <c r="C45" t="n">
         <v>1309.95720885714</v>
       </c>
       <c r="D45" t="n">
-        <v>2097.62504852088</v>
+        <v>2011.0768337519</v>
       </c>
     </row>
     <row r="46">
@@ -1131,13 +1131,13 @@
         <v>48</v>
       </c>
       <c r="B46" t="n">
-        <v>247.259643224212</v>
+        <v>221.115902897825</v>
       </c>
       <c r="C46" t="n">
         <v>544.176543723348</v>
       </c>
       <c r="D46" t="n">
-        <v>913.87324489</v>
+        <v>869.794315577981</v>
       </c>
     </row>
     <row r="47">
@@ -1145,13 +1145,13 @@
         <v>49</v>
       </c>
       <c r="B47" t="n">
-        <v>676.090473839985</v>
+        <v>569.291456582512</v>
       </c>
       <c r="C47" t="n">
         <v>1557.56182306632</v>
       </c>
       <c r="D47" t="n">
-        <v>2789.43877524443</v>
+        <v>2591.78985041937</v>
       </c>
     </row>
     <row r="48">
@@ -1159,13 +1159,13 @@
         <v>50</v>
       </c>
       <c r="B48" t="n">
-        <v>672.834070927464</v>
+        <v>566.526894936938</v>
       </c>
       <c r="C48" t="n">
         <v>1550.49528063082</v>
       </c>
       <c r="D48" t="n">
-        <v>2777.65141680695</v>
+        <v>2579.80000055119</v>
       </c>
     </row>
   </sheetData>

</xml_diff>